<commit_message>
documentacion de funciones wordix
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgb3J5beIylbWJOudmTRe4SqXIbLA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgurVWjh6zKf2PHUBhfcBofZxXVvQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -63,19 +63,37 @@
     <t>indices</t>
   </si>
   <si>
+    <t>↓</t>
+  </si>
+  <si>
     <t>"palabraWordix"</t>
   </si>
   <si>
+    <t>"QUESO"</t>
+  </si>
+  <si>
+    <t>"CASAS"</t>
+  </si>
+  <si>
+    <t>"GOTAS"</t>
+  </si>
+  <si>
+    <t>"PISOS"</t>
+  </si>
+  <si>
+    <t>"MELON"</t>
+  </si>
+  <si>
     <t>"jugador"</t>
   </si>
   <si>
-    <t>majo</t>
-  </si>
-  <si>
-    <t>rudolf</t>
-  </si>
-  <si>
-    <t>pink2000</t>
+    <t>"majo"</t>
+  </si>
+  <si>
+    <t>"rudolf"</t>
+  </si>
+  <si>
+    <t>"pink2000"</t>
   </si>
   <si>
     <t>"intentos"</t>
@@ -129,10 +147,13 @@
     <t>"intento6"</t>
   </si>
   <si>
+    <t>//ejemplos</t>
+  </si>
+  <si>
     <t>Tipo: asociativo</t>
   </si>
   <si>
-    <t>Tipos de datos: Almacena valores Enteros</t>
+    <t>Tipos de datos: Almacena valores Enteros, String</t>
   </si>
   <si>
     <t xml:space="preserve">¿Para qué se utiliza?: Guarda el resumen de UN (1) jugador </t>
@@ -142,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -160,11 +181,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,7 +189,6 @@
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -182,22 +197,31 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color rgb="FF674EA7"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <color rgb="FF6AA84F"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,14 +242,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
-        <bgColor rgb="FFA4C2F4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -236,14 +254,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFC9DAF8"/>
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
     <fill>
@@ -259,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border/>
     <border>
       <left style="thin">
@@ -286,6 +304,31 @@
       </right>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -294,9 +337,17 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -305,6 +356,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -316,14 +370,29 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -332,38 +401,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -372,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -380,148 +417,145 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="8" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="9" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="9" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="13" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -770,427 +804,483 @@
       <c r="G3" s="2">
         <v>5.0</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="J6" s="3"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="18">
+        <v>6.0</v>
+      </c>
+      <c r="C17" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D17" s="22">
+        <v>6.0</v>
+      </c>
+      <c r="E17" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="F17" s="20">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="23">
         <v>0.0</v>
       </c>
-      <c r="D13" s="13">
+      <c r="C18" s="24">
+        <v>14.0</v>
+      </c>
+      <c r="D18" s="25">
+        <v>10.0</v>
+      </c>
+      <c r="E18" s="24">
+        <v>16.0</v>
+      </c>
+      <c r="F18" s="25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="B23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="B24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="B25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="F28" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="32"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="K29" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="38">
         <v>1.0</v>
       </c>
-      <c r="E13" s="14">
+      <c r="D30" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="43">
         <v>2.0</v>
       </c>
-      <c r="F13" s="15">
-        <v>3.0</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="D31" s="43">
+        <v>30.0</v>
+      </c>
+      <c r="E31" s="43">
+        <v>2.0</v>
+      </c>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="45">
+        <v>2.0</v>
+      </c>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="D16" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="E16" s="24">
-        <v>6.0</v>
-      </c>
-      <c r="F16" s="25">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="D17" s="23">
-        <v>14.0</v>
-      </c>
-      <c r="E17" s="24">
+      <c r="M31" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="48">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="48">
         <v>10.0</v>
       </c>
-      <c r="F17" s="25">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="7" t="s">
+      <c r="E32" s="48">
+        <v>1.0</v>
+      </c>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J32" s="48"/>
+      <c r="K32" s="50">
+        <v>1.0</v>
+      </c>
+      <c r="L32" s="51"/>
+      <c r="M32" s="52"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="B34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="F27" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="I28" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="M28" s="38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="40">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="E29" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="44"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="D30" s="12">
-        <v>30.0</v>
-      </c>
-      <c r="E30" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="H30" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="50">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="50">
-        <v>10.0</v>
-      </c>
-      <c r="E31" s="50">
-        <v>1.0</v>
-      </c>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="52">
-        <v>1.0</v>
-      </c>
-      <c r="L31" s="53"/>
-      <c r="M31" s="54"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
+      <c r="B35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1"/>
+      <c r="B36" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>

</xml_diff>